<commit_message>
Some changes on menuprincipal and guiaturistico
</commit_message>
<xml_diff>
--- a/info/ResourceBundle.xlsx
+++ b/info/ResourceBundle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juana\OneDrive\Documentos\GitHub\agenciaDeViajes\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO 5\Documents\GitHub\agenciaDeViajes\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073184F9-6125-424A-9E53-B82E374A778B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2024C4FD-96D0-4133-B12B-5463D3352C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5ACD5306-D8F0-41FA-948E-8F34C9ACE6C0}"/>
   </bookViews>
@@ -26,12 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="381">
   <si>
     <t>CrearReservaController</t>
   </si>
@@ -813,6 +810,375 @@
   </si>
   <si>
     <t>GUIAS MEJOR PUNTUADOS</t>
+  </si>
+  <si>
+    <t>Confirm Your Reservation!</t>
+  </si>
+  <si>
+    <t>Selected Package</t>
+  </si>
+  <si>
+    <t>Travel Date</t>
+  </si>
+  <si>
+    <t>* Remember the range in which it is available</t>
+  </si>
+  <si>
+    <t>From:</t>
+  </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>Number of people</t>
+  </si>
+  <si>
+    <t>* Maximum capacity:</t>
+  </si>
+  <si>
+    <t>Would you like to select a Tour Guide?</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Experience (Hours)</t>
+  </si>
+  <si>
+    <t>Clear Selection</t>
+  </si>
+  <si>
+    <t>Book Now!</t>
+  </si>
+  <si>
+    <t>Destination Detail</t>
+  </si>
+  <si>
+    <t>City:</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Weather:</t>
+  </si>
+  <si>
+    <t>MANAGE DESTINATIONS</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>REMOVE</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>MANAGE GUIDES</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Hours of experience</t>
+  </si>
+  <si>
+    <t>APPLICATIONS</t>
+  </si>
+  <si>
+    <t>MANAGE PACKAGES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration </t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Max C</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Hello again!</t>
+  </si>
+  <si>
+    <t>Welcome back, we have missed you</t>
+  </si>
+  <si>
+    <t>Not registered?</t>
+  </si>
+  <si>
+    <t>Register now</t>
+  </si>
+  <si>
+    <t>Destinations</t>
+  </si>
+  <si>
+    <t>Packages</t>
+  </si>
+  <si>
+    <t>Guides</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Update your information!</t>
+  </si>
+  <si>
+    <t>Update your information and continue enjoying our application.</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package </t>
+  </si>
+  <si>
+    <t>There are %d spaces left!</t>
+  </si>
+  <si>
+    <t>Reserve now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price COP $ $. </t>
+  </si>
+  <si>
+    <t>Additional Services</t>
+  </si>
+  <si>
+    <t>Start date:</t>
+  </si>
+  <si>
+    <t>End Date:</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Veterinarian</t>
+  </si>
+  <si>
+    <t>Pet</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>The best destinations for your pokeadventures</t>
+  </si>
+  <si>
+    <t>Invoice To:</t>
+  </si>
+  <si>
+    <t>Phone:</t>
+  </si>
+  <si>
+    <t>Address:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice: </t>
+  </si>
+  <si>
+    <t>Thank you for your purchase, enjoy your trip</t>
+  </si>
+  <si>
+    <t>txtAddress</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Already registered?</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>ADD DESTINATIONS</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Enter name</t>
+  </si>
+  <si>
+    <t>Enter the city</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>Enter description</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Select images</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>TOUR GUIDE REGISTRATION</t>
+  </si>
+  <si>
+    <t>Your ID:</t>
+  </si>
+  <si>
+    <t>Enter your ID</t>
+  </si>
+  <si>
+    <t>Full Name:</t>
+  </si>
+  <si>
+    <t>Enter your name</t>
+  </si>
+  <si>
+    <t>Hours of experience:</t>
+  </si>
+  <si>
+    <t>Enter experience in hours</t>
+  </si>
+  <si>
+    <t>Image:</t>
+  </si>
+  <si>
+    <t>Select image</t>
+  </si>
+  <si>
+    <t>Selected image:</t>
+  </si>
+  <si>
+    <t>REGISTER</t>
+  </si>
+  <si>
+    <t>PACKAGE REGISTRATION</t>
+  </si>
+  <si>
+    <t>Duration in days:</t>
+  </si>
+  <si>
+    <t>Enter the duration of the package</t>
+  </si>
+  <si>
+    <t>Additional services:</t>
+  </si>
+  <si>
+    <t>Enter the additional services</t>
+  </si>
+  <si>
+    <t>Price in days:</t>
+  </si>
+  <si>
+    <t>Enter the price</t>
+  </si>
+  <si>
+    <t>Maximum quota:</t>
+  </si>
+  <si>
+    <t>Enter the maximum quota</t>
+  </si>
+  <si>
+    <t>Enter the start date of the package</t>
+  </si>
+  <si>
+    <t>End date:</t>
+  </si>
+  <si>
+    <t>Enter the end date of the package</t>
+  </si>
+  <si>
+    <t>Select the destinations that the package will contain</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>WEATHER</t>
+  </si>
+  <si>
+    <t>MANAGE GUIDE REQUESTS</t>
+  </si>
+  <si>
+    <t>ACCEPT</t>
+  </si>
+  <si>
+    <t>DENY</t>
+  </si>
+  <si>
+    <t>STATISTICS</t>
+  </si>
+  <si>
+    <t>MOST BOOKED DESTINATIONS</t>
+  </si>
+  <si>
+    <t>MOST SEARCHED DESTINATIONS</t>
+  </si>
+  <si>
+    <t>TOP RATED GUIDES</t>
+  </si>
+  <si>
+    <t>MOST BOOKED PACKAGES</t>
+  </si>
+  <si>
+    <t>GuiaTuristicoController</t>
+  </si>
+  <si>
+    <t>txtDescription</t>
+  </si>
+  <si>
+    <t>Idiomas Hablados: %s\nExp Horas: %d</t>
+  </si>
+  <si>
+    <t>Languages Spoken: %s\nHours: %d</t>
   </si>
 </sst>
 </file>
@@ -897,8 +1263,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A29758FD-B1B3-44DD-940D-D7130236B3EF}" name="Tabla1" displayName="Tabla1" ref="A2:K162" totalsRowShown="0">
-  <autoFilter ref="A2:K162" xr:uid="{A29758FD-B1B3-44DD-940D-D7130236B3EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A29758FD-B1B3-44DD-940D-D7130236B3EF}" name="Tabla1" displayName="Tabla1" ref="A2:K163" totalsRowShown="0">
+  <autoFilter ref="A2:K163" xr:uid="{A29758FD-B1B3-44DD-940D-D7130236B3EF}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{DB61A800-468E-4337-AB63-C4B3FCA1212A}" name="Controller"/>
     <tableColumn id="2" xr3:uid="{859C3FBF-7B94-4EC0-9049-1A9A7EFB23B5}" name="ID"/>
@@ -1227,11 +1593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD659E6-F76E-49E6-BFF1-9AC73BCA288A}">
-  <dimension ref="A2:K162"/>
+  <dimension ref="A2:K163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J158" sqref="J158"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,7 +1605,7 @@
     <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.21875" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" customWidth="1"/>
     <col min="6" max="6" width="37.6640625" customWidth="1"/>
     <col min="7" max="7" width="47.6640625" customWidth="1"/>
@@ -1298,13 +1664,16 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
+      <c r="E3" t="s">
+        <v>258</v>
+      </c>
       <c r="F3" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblTitle=¡Confirma Tu Reserva!</v>
       </c>
       <c r="G3" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblTitle=</v>
+        <v>CrearReservaController.lblTitle=Confirm Your Reservation!</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1337,13 +1706,16 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
+      <c r="E4" t="s">
+        <v>259</v>
+      </c>
       <c r="F4" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblinfoPackage=Paquete Seleccionado</v>
       </c>
       <c r="G4" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblinfoPackage=</v>
+        <v>CrearReservaController.lblinfoPackage=Selected Package</v>
       </c>
       <c r="H4" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1376,13 +1748,16 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
+      <c r="E5" t="s">
+        <v>260</v>
+      </c>
       <c r="F5" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblFecha=Fecha de Viaje</v>
       </c>
       <c r="G5" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblFecha=</v>
+        <v>CrearReservaController.lblFecha=Travel Date</v>
       </c>
       <c r="H5" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1415,13 +1790,16 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
+      <c r="E6" t="s">
+        <v>261</v>
+      </c>
       <c r="F6" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblRangoDisponible=* Recuerda el rango en el que está disponible</v>
       </c>
       <c r="G6" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblRangoDisponible=</v>
+        <v>CrearReservaController.lblRangoDisponible=* Remember the range in which it is available</v>
       </c>
       <c r="H6" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1454,13 +1832,16 @@
       <c r="D7" t="s">
         <v>20</v>
       </c>
+      <c r="E7" t="s">
+        <v>262</v>
+      </c>
       <c r="F7" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblFechaInicial=Desde:</v>
       </c>
       <c r="G7" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblFechaInicial=</v>
+        <v>CrearReservaController.lblFechaInicial=From:</v>
       </c>
       <c r="H7" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1493,13 +1874,16 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
+      <c r="E8" t="s">
+        <v>263</v>
+      </c>
       <c r="F8" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblFechaFinal=Hasta:</v>
       </c>
       <c r="G8" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblFechaFinal=</v>
+        <v>CrearReservaController.lblFechaFinal=To:</v>
       </c>
       <c r="H8" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1532,13 +1916,16 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
+      <c r="E9" t="s">
+        <v>264</v>
+      </c>
       <c r="F9" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblCant=Cantidad Personas</v>
       </c>
       <c r="G9" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblCant=</v>
+        <v>CrearReservaController.lblCant=Number of people</v>
       </c>
       <c r="H9" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1571,13 +1958,16 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
+      <c r="E10" t="s">
+        <v>265</v>
+      </c>
       <c r="F10" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblCupoMaximo=* Cupo máximo:</v>
       </c>
       <c r="G10" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblCupoMaximo=</v>
+        <v>CrearReservaController.lblCupoMaximo=* Maximum capacity:</v>
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1610,13 +2000,16 @@
       <c r="D11" t="s">
         <v>24</v>
       </c>
+      <c r="E11" t="s">
+        <v>266</v>
+      </c>
       <c r="F11" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.lblGuia=¿Deseas Seleccionar Un Guia Turistico?</v>
       </c>
       <c r="G11" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.lblGuia=</v>
+        <v>CrearReservaController.lblGuia=Would you like to select a Tour Guide?</v>
       </c>
       <c r="H11" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1649,13 +2042,16 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
+      <c r="E12" t="s">
+        <v>267</v>
+      </c>
       <c r="F12" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.clmIdioma=Idiomas</v>
       </c>
       <c r="G12" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.clmIdioma=</v>
+        <v>CrearReservaController.clmIdioma=Languages</v>
       </c>
       <c r="H12" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1688,13 +2084,16 @@
       <c r="D13" t="s">
         <v>26</v>
       </c>
+      <c r="E13" t="s">
+        <v>268</v>
+      </c>
       <c r="F13" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.clmId=Identificacion</v>
       </c>
       <c r="G13" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.clmId=</v>
+        <v>CrearReservaController.clmId=Identity</v>
       </c>
       <c r="H13" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1727,13 +2126,16 @@
       <c r="D14" t="s">
         <v>27</v>
       </c>
+      <c r="E14" t="s">
+        <v>269</v>
+      </c>
       <c r="F14" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.clmName=Nombre</v>
       </c>
       <c r="G14" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.clmName=</v>
+        <v>CrearReservaController.clmName=Name</v>
       </c>
       <c r="H14" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1766,13 +2168,16 @@
       <c r="D15" t="s">
         <v>28</v>
       </c>
+      <c r="E15" t="s">
+        <v>270</v>
+      </c>
       <c r="F15" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.clmExp=Experiencia (Horas)</v>
       </c>
       <c r="G15" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.clmExp=</v>
+        <v>CrearReservaController.clmExp=Experience (Hours)</v>
       </c>
       <c r="H15" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1805,13 +2210,16 @@
       <c r="D16" t="s">
         <v>29</v>
       </c>
+      <c r="E16" t="s">
+        <v>271</v>
+      </c>
       <c r="F16" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.btnLimpiarSeleccion=Limpiar Selección</v>
       </c>
       <c r="G16" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.btnLimpiarSeleccion=</v>
+        <v>CrearReservaController.btnLimpiarSeleccion=Clear Selection</v>
       </c>
       <c r="H16" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1844,13 +2252,16 @@
       <c r="D17" t="s">
         <v>30</v>
       </c>
+      <c r="E17" t="s">
+        <v>272</v>
+      </c>
       <c r="F17" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>CrearReservaController.btnReservar=¡Reserva Ya!</v>
       </c>
       <c r="G17" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>CrearReservaController.btnReservar=</v>
+        <v>CrearReservaController.btnReservar=Book Now!</v>
       </c>
       <c r="H17" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1883,13 +2294,16 @@
       <c r="D18" t="s">
         <v>246</v>
       </c>
+      <c r="E18" t="s">
+        <v>273</v>
+      </c>
       <c r="F18" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>DestinoDetailsController.lblTitle=Detalle Destino</v>
       </c>
       <c r="G18" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>DestinoDetailsController.lblTitle=</v>
+        <v>DestinoDetailsController.lblTitle=Destination Detail</v>
       </c>
       <c r="H18" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1922,13 +2336,16 @@
       <c r="D19" t="s">
         <v>37</v>
       </c>
+      <c r="E19" t="s">
+        <v>274</v>
+      </c>
       <c r="F19" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>DestinoDetailsController.lblCiudad=Ciudad:</v>
       </c>
       <c r="G19" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>DestinoDetailsController.lblCiudad=</v>
+        <v>DestinoDetailsController.lblCiudad=City:</v>
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -1961,13 +2378,16 @@
       <c r="D20" t="s">
         <v>51</v>
       </c>
+      <c r="E20" t="s">
+        <v>275</v>
+      </c>
       <c r="F20" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>DestinoDetailsController.lblDescription=Descripcion</v>
       </c>
       <c r="G20" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>DestinoDetailsController.lblDescription=</v>
+        <v>DestinoDetailsController.lblDescription=Description</v>
       </c>
       <c r="H20" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2000,13 +2420,16 @@
       <c r="D21" t="s">
         <v>39</v>
       </c>
+      <c r="E21" t="s">
+        <v>276</v>
+      </c>
       <c r="F21" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>DestinoDetailsController.lblClima=Clima:</v>
       </c>
       <c r="G21" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>DestinoDetailsController.lblClima=</v>
+        <v>DestinoDetailsController.lblClima=Weather:</v>
       </c>
       <c r="H21" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2039,13 +2462,16 @@
       <c r="D22" t="s">
         <v>41</v>
       </c>
+      <c r="E22" t="s">
+        <v>277</v>
+      </c>
       <c r="F22" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.lblTitle=GESTIONAR DESTINOS</v>
       </c>
       <c r="G22" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.lblTitle=</v>
+        <v>GestionarDestinosController.lblTitle=MANAGE DESTINATIONS</v>
       </c>
       <c r="H22" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2078,13 +2504,16 @@
       <c r="D23" t="s">
         <v>43</v>
       </c>
+      <c r="E23" t="s">
+        <v>278</v>
+      </c>
       <c r="F23" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.txtBuscar=Buscar</v>
       </c>
       <c r="G23" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.txtBuscar=</v>
+        <v>GestionarDestinosController.txtBuscar=Search</v>
       </c>
       <c r="H23" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2117,13 +2546,16 @@
       <c r="D24" t="s">
         <v>45</v>
       </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
       <c r="F24" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.colId=Id</v>
       </c>
       <c r="G24" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.colId=</v>
+        <v>GestionarDestinosController.colId=Id</v>
       </c>
       <c r="H24" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2156,13 +2588,16 @@
       <c r="D25" t="s">
         <v>27</v>
       </c>
+      <c r="E25" t="s">
+        <v>269</v>
+      </c>
       <c r="F25" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.colNombre=Nombre</v>
       </c>
       <c r="G25" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.colNombre=</v>
+        <v>GestionarDestinosController.colNombre=Name</v>
       </c>
       <c r="H25" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2195,13 +2630,16 @@
       <c r="D26" t="s">
         <v>52</v>
       </c>
+      <c r="E26" t="s">
+        <v>279</v>
+      </c>
       <c r="F26" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.colCiudad=Ciudad</v>
       </c>
       <c r="G26" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.colCiudad=</v>
+        <v>GestionarDestinosController.colCiudad=City</v>
       </c>
       <c r="H26" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2234,13 +2672,16 @@
       <c r="D27" t="s">
         <v>51</v>
       </c>
+      <c r="E27" t="s">
+        <v>275</v>
+      </c>
       <c r="F27" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.colDescripcion=Descripcion</v>
       </c>
       <c r="G27" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.colDescripcion=</v>
+        <v>GestionarDestinosController.colDescripcion=Description</v>
       </c>
       <c r="H27" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2273,13 +2714,16 @@
       <c r="D28" t="s">
         <v>50</v>
       </c>
+      <c r="E28" t="s">
+        <v>280</v>
+      </c>
       <c r="F28" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.colClima=Clima</v>
       </c>
       <c r="G28" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.colClima=</v>
+        <v>GestionarDestinosController.colClima=Weather</v>
       </c>
       <c r="H28" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2312,13 +2756,16 @@
       <c r="D29" t="s">
         <v>53</v>
       </c>
+      <c r="E29" t="s">
+        <v>281</v>
+      </c>
       <c r="F29" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.btnEliminar=ELIMINAR</v>
       </c>
       <c r="G29" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.btnEliminar=</v>
+        <v>GestionarDestinosController.btnEliminar=REMOVE</v>
       </c>
       <c r="H29" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2351,13 +2798,16 @@
       <c r="D30" t="s">
         <v>56</v>
       </c>
+      <c r="E30" t="s">
+        <v>282</v>
+      </c>
       <c r="F30" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarDestinosController.btnAgregar=AGREGAR</v>
       </c>
       <c r="G30" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarDestinosController.btnAgregar=</v>
+        <v>GestionarDestinosController.btnAgregar=ADD</v>
       </c>
       <c r="H30" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2390,13 +2840,16 @@
       <c r="D31" t="s">
         <v>58</v>
       </c>
+      <c r="E31" t="s">
+        <v>283</v>
+      </c>
       <c r="F31" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.lblTitle=GESTIONAR GUIAS</v>
       </c>
       <c r="G31" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.lblTitle=</v>
+        <v>GestionarGuiasController.lblTitle=MANAGE GUIDES</v>
       </c>
       <c r="H31" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2429,13 +2882,16 @@
       <c r="D32" t="s">
         <v>43</v>
       </c>
+      <c r="E32" t="s">
+        <v>278</v>
+      </c>
       <c r="F32" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.txtBuscar=Buscar</v>
       </c>
       <c r="G32" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.txtBuscar=</v>
+        <v>GestionarGuiasController.txtBuscar=Search</v>
       </c>
       <c r="H32" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2468,13 +2924,16 @@
       <c r="D33" t="s">
         <v>27</v>
       </c>
+      <c r="E33" t="s">
+        <v>269</v>
+      </c>
       <c r="F33" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.colNombre=Nombre</v>
       </c>
       <c r="G33" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.colNombre=</v>
+        <v>GestionarGuiasController.colNombre=Name</v>
       </c>
       <c r="H33" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2507,13 +2966,16 @@
       <c r="D34" t="s">
         <v>26</v>
       </c>
+      <c r="E34" t="s">
+        <v>284</v>
+      </c>
       <c r="F34" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.colIdentificacion=Identificacion</v>
       </c>
       <c r="G34" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.colIdentificacion=</v>
+        <v>GestionarGuiasController.colIdentificacion=Login</v>
       </c>
       <c r="H34" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2546,13 +3008,16 @@
       <c r="D35" t="s">
         <v>61</v>
       </c>
+      <c r="E35" t="s">
+        <v>285</v>
+      </c>
       <c r="F35" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.colHorasExperiencia=Horas de experiencia</v>
       </c>
       <c r="G35" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.colHorasExperiencia=</v>
+        <v>GestionarGuiasController.colHorasExperiencia=Hours of experience</v>
       </c>
       <c r="H35" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2585,13 +3050,16 @@
       <c r="D36" t="s">
         <v>25</v>
       </c>
+      <c r="E36" t="s">
+        <v>267</v>
+      </c>
       <c r="F36" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.colIdiomas=Idiomas</v>
       </c>
       <c r="G36" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.colIdiomas=</v>
+        <v>GestionarGuiasController.colIdiomas=Languages</v>
       </c>
       <c r="H36" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2624,13 +3092,16 @@
       <c r="D37" t="s">
         <v>53</v>
       </c>
+      <c r="E37" t="s">
+        <v>281</v>
+      </c>
       <c r="F37" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.btnEliminar=ELIMINAR</v>
       </c>
       <c r="G37" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.btnEliminar=</v>
+        <v>GestionarGuiasController.btnEliminar=REMOVE</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2663,13 +3134,16 @@
       <c r="D38" t="s">
         <v>64</v>
       </c>
+      <c r="E38" t="s">
+        <v>286</v>
+      </c>
       <c r="F38" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarGuiasController.btnSolicitudes=SOLICITUDES</v>
       </c>
       <c r="G38" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarGuiasController.btnSolicitudes=</v>
+        <v>GestionarGuiasController.btnSolicitudes=APPLICATIONS</v>
       </c>
       <c r="H38" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2702,13 +3176,16 @@
       <c r="D39" t="s">
         <v>65</v>
       </c>
+      <c r="E39" t="s">
+        <v>287</v>
+      </c>
       <c r="F39" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.lblTitle=GESTIONAR PAQUETES</v>
       </c>
       <c r="G39" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.lblTitle=</v>
+        <v>GestionarPaquetesController.lblTitle=MANAGE PACKAGES</v>
       </c>
       <c r="H39" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2741,13 +3218,16 @@
       <c r="D40" t="s">
         <v>43</v>
       </c>
+      <c r="E40" t="s">
+        <v>278</v>
+      </c>
       <c r="F40" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.txtBuscar=Buscar</v>
       </c>
       <c r="G40" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.txtBuscar=</v>
+        <v>GestionarPaquetesController.txtBuscar=Search</v>
       </c>
       <c r="H40" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2780,13 +3260,16 @@
       <c r="D41" t="s">
         <v>45</v>
       </c>
+      <c r="E41" t="s">
+        <v>45</v>
+      </c>
       <c r="F41" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.colId=Id</v>
       </c>
       <c r="G41" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.colId=</v>
+        <v>GestionarPaquetesController.colId=Id</v>
       </c>
       <c r="H41" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2819,13 +3302,16 @@
       <c r="D42" t="s">
         <v>27</v>
       </c>
+      <c r="E42" t="s">
+        <v>269</v>
+      </c>
       <c r="F42" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.colNombre=Nombre</v>
       </c>
       <c r="G42" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.colNombre=</v>
+        <v>GestionarPaquetesController.colNombre=Name</v>
       </c>
       <c r="H42" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2858,13 +3344,16 @@
       <c r="D43" t="s">
         <v>67</v>
       </c>
+      <c r="E43" t="s">
+        <v>288</v>
+      </c>
       <c r="F43" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v xml:space="preserve">GestionarPaquetesController.colDuracion=Duracion </v>
       </c>
       <c r="G43" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.colDuracion=</v>
+        <v xml:space="preserve">GestionarPaquetesController.colDuracion=Duration </v>
       </c>
       <c r="H43" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2897,13 +3386,16 @@
       <c r="D44" t="s">
         <v>76</v>
       </c>
+      <c r="E44" t="s">
+        <v>289</v>
+      </c>
       <c r="F44" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.colServicios=Servicios</v>
       </c>
       <c r="G44" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.colServicios=</v>
+        <v>GestionarPaquetesController.colServicios=Services</v>
       </c>
       <c r="H44" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2936,13 +3428,16 @@
       <c r="D45" t="s">
         <v>71</v>
       </c>
+      <c r="E45" t="s">
+        <v>290</v>
+      </c>
       <c r="F45" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.colCupoMaximo=C Maximo</v>
       </c>
       <c r="G45" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.colCupoMaximo=</v>
+        <v>GestionarPaquetesController.colCupoMaximo=Max C</v>
       </c>
       <c r="H45" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -2975,13 +3470,16 @@
       <c r="D46" t="s">
         <v>73</v>
       </c>
+      <c r="E46" t="s">
+        <v>291</v>
+      </c>
       <c r="F46" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.colFechaInicio=Fecha inicio</v>
       </c>
       <c r="G46" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.colFechaInicio=</v>
+        <v>GestionarPaquetesController.colFechaInicio=Start Date</v>
       </c>
       <c r="H46" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3014,13 +3512,16 @@
       <c r="D47" t="s">
         <v>75</v>
       </c>
+      <c r="E47" t="s">
+        <v>292</v>
+      </c>
       <c r="F47" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>GestionarPaquetesController.colFechaFin=Fecha fin</v>
       </c>
       <c r="G47" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>GestionarPaquetesController.colFechaFin=</v>
+        <v>GestionarPaquetesController.colFechaFin=End Date</v>
       </c>
       <c r="H47" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3053,13 +3554,16 @@
       <c r="D48" t="s">
         <v>79</v>
       </c>
+      <c r="E48" t="s">
+        <v>293</v>
+      </c>
       <c r="F48" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>LoginController.lblTitle=¡Hola de nuevo!</v>
       </c>
       <c r="G48" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>LoginController.lblTitle=</v>
+        <v>LoginController.lblTitle=Hello again!</v>
       </c>
       <c r="H48" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3092,13 +3596,16 @@
       <c r="D49" t="s">
         <v>80</v>
       </c>
+      <c r="E49" t="s">
+        <v>294</v>
+      </c>
       <c r="F49" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>LoginController.lblInfo=Bienvenido de nuevo, te hemos extrañado</v>
       </c>
       <c r="G49" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>LoginController.lblInfo=</v>
+        <v>LoginController.lblInfo=Welcome back, we have missed you</v>
       </c>
       <c r="H49" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3131,13 +3638,16 @@
       <c r="D50" t="s">
         <v>26</v>
       </c>
+      <c r="E50" t="s">
+        <v>284</v>
+      </c>
       <c r="F50" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>LoginController.txtEmail=Identificacion</v>
       </c>
       <c r="G50" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>LoginController.txtEmail=</v>
+        <v>LoginController.txtEmail=Login</v>
       </c>
       <c r="H50" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3170,13 +3680,16 @@
       <c r="D51" t="s">
         <v>83</v>
       </c>
+      <c r="E51" t="s">
+        <v>103</v>
+      </c>
       <c r="F51" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>LoginController.txtPassword=Contraseña</v>
       </c>
       <c r="G51" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>LoginController.txtPassword=</v>
+        <v>LoginController.txtPassword=Password</v>
       </c>
       <c r="H51" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3209,13 +3722,16 @@
       <c r="D52" t="s">
         <v>85</v>
       </c>
+      <c r="E52" t="s">
+        <v>284</v>
+      </c>
       <c r="F52" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>LoginController.btnIniciar=Iniciar Sesión</v>
       </c>
       <c r="G52" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>LoginController.btnIniciar=</v>
+        <v>LoginController.btnIniciar=Login</v>
       </c>
       <c r="H52" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3248,13 +3764,16 @@
       <c r="D53" t="s">
         <v>86</v>
       </c>
+      <c r="E53" t="s">
+        <v>295</v>
+      </c>
       <c r="F53" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>LoginController.lblNoRegistrado=¿No esta registrado?</v>
       </c>
       <c r="G53" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>LoginController.lblNoRegistrado=</v>
+        <v>LoginController.lblNoRegistrado=Not registered?</v>
       </c>
       <c r="H53" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3287,13 +3806,16 @@
       <c r="D54" t="s">
         <v>89</v>
       </c>
+      <c r="E54" t="s">
+        <v>296</v>
+      </c>
       <c r="F54" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>LoginController.btnRegistrar=Registrarse ahora</v>
       </c>
       <c r="G54" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>LoginController.btnRegistrar=</v>
+        <v>LoginController.btnRegistrar=Register now</v>
       </c>
       <c r="H54" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3326,13 +3848,16 @@
       <c r="D55" t="s">
         <v>95</v>
       </c>
+      <c r="E55" t="s">
+        <v>297</v>
+      </c>
       <c r="F55" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>MainMenuController.lblBtnDestinos=Destinos</v>
       </c>
       <c r="G55" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>MainMenuController.lblBtnDestinos=</v>
+        <v>MainMenuController.lblBtnDestinos=Destinations</v>
       </c>
       <c r="H55" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3365,13 +3890,16 @@
       <c r="D56" t="s">
         <v>94</v>
       </c>
+      <c r="E56" t="s">
+        <v>298</v>
+      </c>
       <c r="F56" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>MainMenuController.lblbtnPaquetes=Paquetes</v>
       </c>
       <c r="G56" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>MainMenuController.lblbtnPaquetes=</v>
+        <v>MainMenuController.lblbtnPaquetes=Packages</v>
       </c>
       <c r="H56" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3404,13 +3932,16 @@
       <c r="D57" t="s">
         <v>93</v>
       </c>
+      <c r="E57" t="s">
+        <v>299</v>
+      </c>
       <c r="F57" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>MainMenuController.lblBtnGuias=Guias</v>
       </c>
       <c r="G57" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>MainMenuController.lblBtnGuias=</v>
+        <v>MainMenuController.lblBtnGuias=Guides</v>
       </c>
       <c r="H57" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3443,13 +3974,16 @@
       <c r="D58" t="s">
         <v>95</v>
       </c>
+      <c r="E58" t="s">
+        <v>297</v>
+      </c>
       <c r="F58" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>MenuPrincipalAdminController.lblBtnDestinos=Destinos</v>
       </c>
       <c r="G58" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>MenuPrincipalAdminController.lblBtnDestinos=</v>
+        <v>MenuPrincipalAdminController.lblBtnDestinos=Destinations</v>
       </c>
       <c r="H58" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3482,13 +4016,16 @@
       <c r="D59" t="s">
         <v>94</v>
       </c>
+      <c r="E59" t="s">
+        <v>298</v>
+      </c>
       <c r="F59" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>MenuPrincipalAdminController.lblbtnPaquetes=Paquetes</v>
       </c>
       <c r="G59" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>MenuPrincipalAdminController.lblbtnPaquetes=</v>
+        <v>MenuPrincipalAdminController.lblbtnPaquetes=Packages</v>
       </c>
       <c r="H59" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3521,13 +4058,16 @@
       <c r="D60" t="s">
         <v>93</v>
       </c>
+      <c r="E60" t="s">
+        <v>299</v>
+      </c>
       <c r="F60" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>MenuPrincipalAdminController.lblBtnGuias=Guias</v>
       </c>
       <c r="G60" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>MenuPrincipalAdminController.lblBtnGuias=</v>
+        <v>MenuPrincipalAdminController.lblBtnGuias=Guides</v>
       </c>
       <c r="H60" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3560,13 +4100,16 @@
       <c r="D61" t="s">
         <v>97</v>
       </c>
+      <c r="E61" t="s">
+        <v>300</v>
+      </c>
       <c r="F61" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>MenuPrincipalAdminController.lblBtnClientes=Clientes</v>
       </c>
       <c r="G61" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>MenuPrincipalAdminController.lblBtnClientes=</v>
+        <v>MenuPrincipalAdminController.lblBtnClientes=Customers</v>
       </c>
       <c r="H61" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3599,13 +4142,16 @@
       <c r="D62" t="s">
         <v>100</v>
       </c>
+      <c r="E62" t="s">
+        <v>301</v>
+      </c>
       <c r="F62" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.lblTitle=¡Actualiza tu informacion!</v>
       </c>
       <c r="G62" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.lblTitle=</v>
+        <v>ModificarClienteController.lblTitle=Update your information!</v>
       </c>
       <c r="H62" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3638,13 +4184,16 @@
       <c r="D63" t="s">
         <v>101</v>
       </c>
+      <c r="E63" t="s">
+        <v>302</v>
+      </c>
       <c r="F63" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.lblInfo=Actualiza tus datos y continua disfrutando de nuestra aplicacion</v>
       </c>
       <c r="G63" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.lblInfo=</v>
+        <v>ModificarClienteController.lblInfo=Update your information and continue enjoying our application.</v>
       </c>
       <c r="H63" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3677,13 +4226,16 @@
       <c r="D64" t="s">
         <v>26</v>
       </c>
+      <c r="E64" t="s">
+        <v>284</v>
+      </c>
       <c r="F64" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.txtIdentificacion=Identificacion</v>
       </c>
       <c r="G64" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.txtIdentificacion=</v>
+        <v>ModificarClienteController.txtIdentificacion=Login</v>
       </c>
       <c r="H64" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3716,13 +4268,16 @@
       <c r="D65" t="s">
         <v>102</v>
       </c>
+      <c r="E65" t="s">
+        <v>303</v>
+      </c>
       <c r="F65" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.txtNombre=Nombre Completo</v>
       </c>
       <c r="G65" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.txtNombre=</v>
+        <v>ModificarClienteController.txtNombre=Full Name</v>
       </c>
       <c r="H65" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3755,13 +4310,16 @@
       <c r="D66" t="s">
         <v>103</v>
       </c>
+      <c r="E66" t="s">
+        <v>103</v>
+      </c>
       <c r="F66" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.txtPassword=Password</v>
       </c>
       <c r="G66" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.txtPassword=</v>
+        <v>ModificarClienteController.txtPassword=Password</v>
       </c>
       <c r="H66" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3794,13 +4352,16 @@
       <c r="D67" t="s">
         <v>104</v>
       </c>
+      <c r="E67" t="s">
+        <v>104</v>
+      </c>
       <c r="F67" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.txtEmail=Email</v>
       </c>
       <c r="G67" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.txtEmail=</v>
+        <v>ModificarClienteController.txtEmail=Email</v>
       </c>
       <c r="H67" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3833,13 +4394,16 @@
       <c r="D68" t="s">
         <v>154</v>
       </c>
+      <c r="E68" t="s">
+        <v>304</v>
+      </c>
       <c r="F68" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.txtTelefono=Teléfono</v>
       </c>
       <c r="G68" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.txtTelefono=</v>
+        <v>ModificarClienteController.txtTelefono=Phone</v>
       </c>
       <c r="H68" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3872,13 +4436,16 @@
       <c r="D69" t="s">
         <v>105</v>
       </c>
+      <c r="E69" t="s">
+        <v>305</v>
+      </c>
       <c r="F69" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.txtDireccion=Direccion</v>
       </c>
       <c r="G69" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.txtDireccion=</v>
+        <v>ModificarClienteController.txtDireccion=Address</v>
       </c>
       <c r="H69" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3911,13 +4478,16 @@
       <c r="D70" t="s">
         <v>106</v>
       </c>
+      <c r="E70" t="s">
+        <v>306</v>
+      </c>
       <c r="F70" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ModificarClienteController.btnActualizar=Actualizar</v>
       </c>
       <c r="G70" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ModificarClienteController.btnActualizar=</v>
+        <v>ModificarClienteController.btnActualizar=Update</v>
       </c>
       <c r="H70" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3950,13 +4520,16 @@
       <c r="D71" t="s">
         <v>113</v>
       </c>
+      <c r="E71" t="s">
+        <v>307</v>
+      </c>
       <c r="F71" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v xml:space="preserve">PaqueteDetailsController.lblPaquete=Paquete </v>
       </c>
       <c r="G71" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.lblPaquete=</v>
+        <v xml:space="preserve">PaqueteDetailsController.lblPaquete=Package </v>
       </c>
       <c r="H71" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -3989,13 +4562,16 @@
       <c r="D72" t="s">
         <v>124</v>
       </c>
+      <c r="E72" t="s">
+        <v>308</v>
+      </c>
       <c r="F72" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PaqueteDetailsController.lblInfoCupos=¡Quedan %d cupos!</v>
       </c>
       <c r="G72" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.lblInfoCupos=</v>
+        <v>PaqueteDetailsController.lblInfoCupos=There are %d spaces left!</v>
       </c>
       <c r="H72" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4028,13 +4604,16 @@
       <c r="D73" t="s">
         <v>116</v>
       </c>
+      <c r="E73" t="s">
+        <v>309</v>
+      </c>
       <c r="F73" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PaqueteDetailsController.btnReservar=Reserva ahora</v>
       </c>
       <c r="G73" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.btnReservar=</v>
+        <v>PaqueteDetailsController.btnReservar=Reserve now</v>
       </c>
       <c r="H73" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4067,13 +4646,16 @@
       <c r="D74" t="s">
         <v>117</v>
       </c>
+      <c r="E74" t="s">
+        <v>310</v>
+      </c>
       <c r="F74" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v xml:space="preserve">PaqueteDetailsController.lblPrecio=Precio COP $ </v>
       </c>
       <c r="G74" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.lblPrecio=</v>
+        <v xml:space="preserve">PaqueteDetailsController.lblPrecio=Price COP $ $. </v>
       </c>
       <c r="H74" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4106,13 +4688,16 @@
       <c r="D75" t="s">
         <v>123</v>
       </c>
+      <c r="E75" t="s">
+        <v>311</v>
+      </c>
       <c r="F75" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PaqueteDetailsController.lblServiciosExtra=Servicios Adicionales</v>
       </c>
       <c r="G75" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.lblServiciosExtra=</v>
+        <v>PaqueteDetailsController.lblServiciosExtra=Additional Services</v>
       </c>
       <c r="H75" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4145,13 +4730,16 @@
       <c r="D76" t="s">
         <v>95</v>
       </c>
+      <c r="E76" t="s">
+        <v>297</v>
+      </c>
       <c r="F76" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PaqueteDetailsController.lblDestinos=Destinos</v>
       </c>
       <c r="G76" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.lblDestinos=</v>
+        <v>PaqueteDetailsController.lblDestinos=Destinations</v>
       </c>
       <c r="H76" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4184,13 +4772,16 @@
       <c r="D77" t="s">
         <v>120</v>
       </c>
+      <c r="E77" t="s">
+        <v>312</v>
+      </c>
       <c r="F77" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PaqueteDetailsController.lblFechaInicial=Fecha Inicial:</v>
       </c>
       <c r="G77" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.lblFechaInicial=</v>
+        <v>PaqueteDetailsController.lblFechaInicial=Start date:</v>
       </c>
       <c r="H77" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4223,13 +4814,16 @@
       <c r="D78" t="s">
         <v>121</v>
       </c>
+      <c r="E78" t="s">
+        <v>313</v>
+      </c>
       <c r="F78" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PaqueteDetailsController.lblFechaFinal=Fecha Final:</v>
       </c>
       <c r="G78" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PaqueteDetailsController.lblFechaFinal=</v>
+        <v>PaqueteDetailsController.lblFechaFinal=End Date:</v>
       </c>
       <c r="H78" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4262,13 +4856,16 @@
       <c r="D79" t="s">
         <v>146</v>
       </c>
+      <c r="E79" t="s">
+        <v>314</v>
+      </c>
       <c r="F79" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblEstado=Estado</v>
       </c>
       <c r="G79" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblEstado=</v>
+        <v>PDFFacturaController.lblEstado=Status</v>
       </c>
       <c r="H79" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4301,13 +4898,16 @@
       <c r="D80" t="s">
         <v>145</v>
       </c>
+      <c r="E80" t="s">
+        <v>315</v>
+      </c>
       <c r="F80" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblVeterinario=Veterinario</v>
       </c>
       <c r="G80" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblVeterinario=</v>
+        <v>PDFFacturaController.lblVeterinario=Veterinarian</v>
       </c>
       <c r="H80" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4340,13 +4940,16 @@
       <c r="D81" t="s">
         <v>144</v>
       </c>
+      <c r="E81" t="s">
+        <v>316</v>
+      </c>
       <c r="F81" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblMascota=Mascota</v>
       </c>
       <c r="G81" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblMascota=</v>
+        <v>PDFFacturaController.lblMascota=Pet</v>
       </c>
       <c r="H81" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4379,13 +4982,16 @@
       <c r="D82" t="s">
         <v>143</v>
       </c>
+      <c r="E82" t="s">
+        <v>317</v>
+      </c>
       <c r="F82" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblTipo=Tipo</v>
       </c>
       <c r="G82" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblTipo=</v>
+        <v>PDFFacturaController.lblTipo=Type</v>
       </c>
       <c r="H82" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4418,13 +5024,16 @@
       <c r="D83" t="s">
         <v>142</v>
       </c>
+      <c r="E83" t="s">
+        <v>318</v>
+      </c>
       <c r="F83" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblSexo=Sexo</v>
       </c>
       <c r="G83" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblSexo=</v>
+        <v>PDFFacturaController.lblSexo=Sex</v>
       </c>
       <c r="H83" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4457,13 +5066,16 @@
       <c r="D84" t="s">
         <v>141</v>
       </c>
+      <c r="E84" t="s">
+        <v>319</v>
+      </c>
       <c r="F84" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblDiagnostico=Diagnostico</v>
       </c>
       <c r="G84" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblDiagnostico=</v>
+        <v>PDFFacturaController.lblDiagnostico=Diagnosis</v>
       </c>
       <c r="H84" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4496,13 +5108,16 @@
       <c r="D85" t="s">
         <v>140</v>
       </c>
+      <c r="E85" t="s">
+        <v>320</v>
+      </c>
       <c r="F85" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblTratamiento=Tratamiento</v>
       </c>
       <c r="G85" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblTratamiento=</v>
+        <v>PDFFacturaController.lblTratamiento=Treatment</v>
       </c>
       <c r="H85" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4535,13 +5150,16 @@
       <c r="D86" t="s">
         <v>139</v>
       </c>
+      <c r="E86" t="s">
+        <v>321</v>
+      </c>
       <c r="F86" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblPrecio=Precio</v>
       </c>
       <c r="G86" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblPrecio=</v>
+        <v>PDFFacturaController.lblPrecio=Price</v>
       </c>
       <c r="H86" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4574,13 +5192,16 @@
       <c r="D87" t="s">
         <v>138</v>
       </c>
+      <c r="E87" t="s">
+        <v>322</v>
+      </c>
       <c r="F87" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblLema=Los mejores destinos para tus pokeaventuras</v>
       </c>
       <c r="G87" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblLema=</v>
+        <v>PDFFacturaController.lblLema=The best destinations for your pokeadventures</v>
       </c>
       <c r="H87" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4613,13 +5234,16 @@
       <c r="D88" t="s">
         <v>147</v>
       </c>
+      <c r="E88" t="s">
+        <v>323</v>
+      </c>
       <c r="F88" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblFacturaPara=Factura Para:</v>
       </c>
       <c r="G88" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblFacturaPara=</v>
+        <v>PDFFacturaController.lblFacturaPara=Invoice To:</v>
       </c>
       <c r="H88" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4652,13 +5276,16 @@
       <c r="D89" t="s">
         <v>148</v>
       </c>
+      <c r="E89" t="s">
+        <v>324</v>
+      </c>
       <c r="F89" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblTelefono=Telefono:</v>
       </c>
       <c r="G89" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblTelefono=</v>
+        <v>PDFFacturaController.lblTelefono=Phone:</v>
       </c>
       <c r="H89" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4691,13 +5318,16 @@
       <c r="D90" t="s">
         <v>149</v>
       </c>
+      <c r="E90" t="s">
+        <v>325</v>
+      </c>
       <c r="F90" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblDireccion=Direccion:</v>
       </c>
       <c r="G90" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblDireccion=</v>
+        <v>PDFFacturaController.lblDireccion=Address:</v>
       </c>
       <c r="H90" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4730,13 +5360,16 @@
       <c r="D91" t="s">
         <v>151</v>
       </c>
+      <c r="E91" t="s">
+        <v>326</v>
+      </c>
       <c r="F91" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v xml:space="preserve">PDFFacturaController.lblFactura=Factura: </v>
       </c>
       <c r="G91" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblFactura=</v>
+        <v xml:space="preserve">PDFFacturaController.lblFactura=Invoice: </v>
       </c>
       <c r="H91" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4769,13 +5402,16 @@
       <c r="D92" t="s">
         <v>153</v>
       </c>
+      <c r="E92" t="s">
+        <v>327</v>
+      </c>
       <c r="F92" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>PDFFacturaController.lblThx=Gracias por tu compra, disfruta tu viaje</v>
       </c>
       <c r="G92" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>PDFFacturaController.lblThx=</v>
+        <v>PDFFacturaController.lblThx=Thank you for your purchase, enjoy your trip</v>
       </c>
       <c r="H92" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4808,13 +5444,16 @@
       <c r="D93" t="s">
         <v>26</v>
       </c>
+      <c r="E93" t="s">
+        <v>284</v>
+      </c>
       <c r="F93" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.txtIdentificacion=Identificacion</v>
       </c>
       <c r="G93" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.txtIdentificacion=</v>
+        <v>RegistrationController.txtIdentificacion=Login</v>
       </c>
       <c r="H93" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4847,13 +5486,16 @@
       <c r="D94" t="s">
         <v>102</v>
       </c>
+      <c r="E94" t="s">
+        <v>303</v>
+      </c>
       <c r="F94" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.txtNombre=Nombre Completo</v>
       </c>
       <c r="G94" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.txtNombre=</v>
+        <v>RegistrationController.txtNombre=Full Name</v>
       </c>
       <c r="H94" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4886,13 +5528,16 @@
       <c r="D95" t="s">
         <v>83</v>
       </c>
+      <c r="E95" t="s">
+        <v>103</v>
+      </c>
       <c r="F95" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.txtPassword=Contraseña</v>
       </c>
       <c r="G95" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.txtPassword=</v>
+        <v>RegistrationController.txtPassword=Password</v>
       </c>
       <c r="H95" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4925,13 +5570,16 @@
       <c r="D96" t="s">
         <v>104</v>
       </c>
+      <c r="E96" t="s">
+        <v>104</v>
+      </c>
       <c r="F96" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.txtEmail=Email</v>
       </c>
       <c r="G96" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.txtEmail=</v>
+        <v>RegistrationController.txtEmail=Email</v>
       </c>
       <c r="H96" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -4964,13 +5612,16 @@
       <c r="D97" t="s">
         <v>154</v>
       </c>
+      <c r="E97" t="s">
+        <v>304</v>
+      </c>
       <c r="F97" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.txtTelefono=Teléfono</v>
       </c>
       <c r="G97" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.txtTelefono=</v>
+        <v>RegistrationController.txtTelefono=Phone</v>
       </c>
       <c r="H97" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5003,13 +5654,16 @@
       <c r="D98" t="s">
         <v>108</v>
       </c>
+      <c r="E98" t="s">
+        <v>328</v>
+      </c>
       <c r="F98" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.txtDireccion=txtDireccion</v>
       </c>
       <c r="G98" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.txtDireccion=</v>
+        <v>RegistrationController.txtDireccion=txtAddress</v>
       </c>
       <c r="H98" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5042,13 +5696,16 @@
       <c r="D99" t="s">
         <v>155</v>
       </c>
+      <c r="E99" t="s">
+        <v>329</v>
+      </c>
       <c r="F99" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.btnRegistro=Registrarse</v>
       </c>
       <c r="G99" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.btnRegistro=</v>
+        <v>RegistrationController.btnRegistro=Register</v>
       </c>
       <c r="H99" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5081,13 +5738,16 @@
       <c r="D100" t="s">
         <v>159</v>
       </c>
+      <c r="E100" t="s">
+        <v>330</v>
+      </c>
       <c r="F100" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.lblYaRegistrado=¿Ya te registraste?</v>
       </c>
       <c r="G100" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.lblYaRegistrado=</v>
+        <v>RegistrationController.lblYaRegistrado=Already registered?</v>
       </c>
       <c r="H100" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5120,13 +5780,16 @@
       <c r="D101" t="s">
         <v>158</v>
       </c>
+      <c r="E101" t="s">
+        <v>331</v>
+      </c>
       <c r="F101" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistrationController.btnLogin=Iniciar sesión</v>
       </c>
       <c r="G101" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistrationController.btnLogin=</v>
+        <v>RegistrationController.btnLogin=Sign in</v>
       </c>
       <c r="H101" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5159,13 +5822,16 @@
       <c r="D102" t="s">
         <v>168</v>
       </c>
+      <c r="E102" t="s">
+        <v>332</v>
+      </c>
       <c r="F102" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.lblTitulo=AGREGAR DESTINOS</v>
       </c>
       <c r="G102" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.lblTitulo=</v>
+        <v>RegistroDestinoController.lblTitulo=ADD DESTINATIONS</v>
       </c>
       <c r="H102" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5198,13 +5864,16 @@
       <c r="D103" t="s">
         <v>169</v>
       </c>
+      <c r="E103" t="s">
+        <v>333</v>
+      </c>
       <c r="F103" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.lblNombre=Nombre:</v>
       </c>
       <c r="G103" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.lblNombre=</v>
+        <v>RegistroDestinoController.lblNombre=Name:</v>
       </c>
       <c r="H103" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5237,13 +5906,16 @@
       <c r="D104" t="s">
         <v>174</v>
       </c>
+      <c r="E104" t="s">
+        <v>334</v>
+      </c>
       <c r="F104" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.txtNombre=Ingrese el nombre</v>
       </c>
       <c r="G104" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.txtNombre=</v>
+        <v>RegistroDestinoController.txtNombre=Enter name</v>
       </c>
       <c r="H104" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5276,13 +5948,16 @@
       <c r="D105" t="s">
         <v>37</v>
       </c>
+      <c r="E105" t="s">
+        <v>274</v>
+      </c>
       <c r="F105" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.lblCiudad=Ciudad:</v>
       </c>
       <c r="G105" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.lblCiudad=</v>
+        <v>RegistroDestinoController.lblCiudad=City:</v>
       </c>
       <c r="H105" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5315,13 +5990,16 @@
       <c r="D106" t="s">
         <v>173</v>
       </c>
+      <c r="E106" t="s">
+        <v>335</v>
+      </c>
       <c r="F106" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.txtCiudad=Ingrese la ciudad</v>
       </c>
       <c r="G106" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.txtCiudad=</v>
+        <v>RegistroDestinoController.txtCiudad=Enter the city</v>
       </c>
       <c r="H106" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5354,13 +6032,16 @@
       <c r="D107" t="s">
         <v>170</v>
       </c>
+      <c r="E107" t="s">
+        <v>336</v>
+      </c>
       <c r="F107" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.lblDescripcion=Descripcion:</v>
       </c>
       <c r="G107" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.lblDescripcion=</v>
+        <v>RegistroDestinoController.lblDescripcion=Description:</v>
       </c>
       <c r="H107" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5393,13 +6074,16 @@
       <c r="D108" t="s">
         <v>172</v>
       </c>
+      <c r="E108" t="s">
+        <v>337</v>
+      </c>
       <c r="F108" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.txtDescripcion=Ingrese la descripcion</v>
       </c>
       <c r="G108" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.txtDescripcion=</v>
+        <v>RegistroDestinoController.txtDescripcion=Enter description</v>
       </c>
       <c r="H108" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5432,13 +6116,16 @@
       <c r="D109" t="s">
         <v>39</v>
       </c>
+      <c r="E109" t="s">
+        <v>276</v>
+      </c>
       <c r="F109" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.lblClima=Clima:</v>
       </c>
       <c r="G109" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.lblClima=</v>
+        <v>RegistroDestinoController.lblClima=Weather:</v>
       </c>
       <c r="H109" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5471,13 +6158,16 @@
       <c r="D110" t="s">
         <v>171</v>
       </c>
+      <c r="E110" t="s">
+        <v>338</v>
+      </c>
       <c r="F110" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.cbClima=Seleccionar</v>
       </c>
       <c r="G110" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.cbClima=</v>
+        <v>RegistroDestinoController.cbClima=Select</v>
       </c>
       <c r="H110" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5510,13 +6200,16 @@
       <c r="D111" t="s">
         <v>175</v>
       </c>
+      <c r="E111" t="s">
+        <v>339</v>
+      </c>
       <c r="F111" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.lblSeleccionarImagen=Seleccionar imagenes</v>
       </c>
       <c r="G111" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.lblSeleccionarImagen=</v>
+        <v>RegistroDestinoController.lblSeleccionarImagen=Select images</v>
       </c>
       <c r="H111" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5549,13 +6242,16 @@
       <c r="D112" t="s">
         <v>176</v>
       </c>
+      <c r="E112" t="s">
+        <v>340</v>
+      </c>
       <c r="F112" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.btnSeleccionar=SELECCIONAR</v>
       </c>
       <c r="G112" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.btnSeleccionar=</v>
+        <v>RegistroDestinoController.btnSeleccionar=SELECT</v>
       </c>
       <c r="H112" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5588,13 +6284,16 @@
       <c r="D113" t="s">
         <v>56</v>
       </c>
+      <c r="E113" t="s">
+        <v>282</v>
+      </c>
       <c r="F113" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroDestinoController.btnAgregar=AGREGAR</v>
       </c>
       <c r="G113" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroDestinoController.btnAgregar=</v>
+        <v>RegistroDestinoController.btnAgregar=ADD</v>
       </c>
       <c r="H113" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5627,13 +6326,16 @@
       <c r="D114" t="s">
         <v>180</v>
       </c>
+      <c r="E114" t="s">
+        <v>341</v>
+      </c>
       <c r="F114" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.lblTitle=REGISTRO DE GUIA TURISTICO</v>
       </c>
       <c r="G114" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.lblTitle=</v>
+        <v>RegistroGuiaController.lblTitle=TOUR GUIDE REGISTRATION</v>
       </c>
       <c r="H114" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5666,13 +6368,16 @@
       <c r="D115" t="s">
         <v>181</v>
       </c>
+      <c r="E115" t="s">
+        <v>342</v>
+      </c>
       <c r="F115" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.lblIdentificacion=Identificacion:</v>
       </c>
       <c r="G115" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.lblIdentificacion=</v>
+        <v>RegistroGuiaController.lblIdentificacion=Your ID:</v>
       </c>
       <c r="H115" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5705,13 +6410,16 @@
       <c r="D116" t="s">
         <v>183</v>
       </c>
+      <c r="E116" t="s">
+        <v>343</v>
+      </c>
       <c r="F116" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.txtIdentificacion=Ingrese su identificacion</v>
       </c>
       <c r="G116" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.txtIdentificacion=</v>
+        <v>RegistroGuiaController.txtIdentificacion=Enter your ID</v>
       </c>
       <c r="H116" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5744,13 +6452,16 @@
       <c r="D117" t="s">
         <v>182</v>
       </c>
+      <c r="E117" t="s">
+        <v>344</v>
+      </c>
       <c r="F117" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.lblNombre=Nombre completo:</v>
       </c>
       <c r="G117" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.lblNombre=</v>
+        <v>RegistroGuiaController.lblNombre=Full Name:</v>
       </c>
       <c r="H117" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5783,13 +6494,16 @@
       <c r="D118" t="s">
         <v>184</v>
       </c>
+      <c r="E118" t="s">
+        <v>345</v>
+      </c>
       <c r="F118" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.txtNombre=Ingrese su nombre</v>
       </c>
       <c r="G118" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.txtNombre=</v>
+        <v>RegistroGuiaController.txtNombre=Enter your name</v>
       </c>
       <c r="H118" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5822,13 +6536,16 @@
       <c r="D119" t="s">
         <v>186</v>
       </c>
+      <c r="E119" t="s">
+        <v>346</v>
+      </c>
       <c r="F119" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.lblHoras=Horas de experiencia:</v>
       </c>
       <c r="G119" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.lblHoras=</v>
+        <v>RegistroGuiaController.lblHoras=Hours of experience:</v>
       </c>
       <c r="H119" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5861,13 +6578,16 @@
       <c r="D120" t="s">
         <v>185</v>
       </c>
+      <c r="E120" t="s">
+        <v>347</v>
+      </c>
       <c r="F120" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.txtHoras=Ingrese la experiencia en horas</v>
       </c>
       <c r="G120" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.txtHoras=</v>
+        <v>RegistroGuiaController.txtHoras=Enter experience in hours</v>
       </c>
       <c r="H120" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5900,13 +6620,16 @@
       <c r="D121" t="s">
         <v>187</v>
       </c>
+      <c r="E121" t="s">
+        <v>348</v>
+      </c>
       <c r="F121" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.lblImagen=Imagen:</v>
       </c>
       <c r="G121" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.lblImagen=</v>
+        <v>RegistroGuiaController.lblImagen=Image:</v>
       </c>
       <c r="H121" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5939,13 +6662,16 @@
       <c r="D122" t="s">
         <v>188</v>
       </c>
+      <c r="E122" t="s">
+        <v>349</v>
+      </c>
       <c r="F122" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.btnImagen=Seleccionar imagen</v>
       </c>
       <c r="G122" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.btnImagen=</v>
+        <v>RegistroGuiaController.btnImagen=Select image</v>
       </c>
       <c r="H122" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -5978,13 +6704,16 @@
       <c r="D123" t="s">
         <v>189</v>
       </c>
+      <c r="E123" t="s">
+        <v>350</v>
+      </c>
       <c r="F123" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.lblImagenSeleccionada=Imagen seleccionada:</v>
       </c>
       <c r="G123" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.lblImagenSeleccionada=</v>
+        <v>RegistroGuiaController.lblImagenSeleccionada=Selected image:</v>
       </c>
       <c r="H123" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6017,13 +6746,16 @@
       <c r="D124" t="s">
         <v>196</v>
       </c>
+      <c r="E124" t="s">
+        <v>351</v>
+      </c>
       <c r="F124" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroGuiaController.btnRegistrar=REGISTRAR</v>
       </c>
       <c r="G124" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroGuiaController.btnRegistrar=</v>
+        <v>RegistroGuiaController.btnRegistrar=REGISTER</v>
       </c>
       <c r="H124" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6056,13 +6788,16 @@
       <c r="D125" t="s">
         <v>197</v>
       </c>
+      <c r="E125" t="s">
+        <v>352</v>
+      </c>
       <c r="F125" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblTitulo=REGISTRO DE PAQUETES</v>
       </c>
       <c r="G125" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblTitulo=</v>
+        <v>RegistroPaquetesController.lblTitulo=PACKAGE REGISTRATION</v>
       </c>
       <c r="H125" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6095,13 +6830,16 @@
       <c r="D126" t="s">
         <v>169</v>
       </c>
+      <c r="E126" t="s">
+        <v>333</v>
+      </c>
       <c r="F126" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblNombre=Nombre:</v>
       </c>
       <c r="G126" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblNombre=</v>
+        <v>RegistroPaquetesController.lblNombre=Name:</v>
       </c>
       <c r="H126" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6134,13 +6872,16 @@
       <c r="D127" t="s">
         <v>174</v>
       </c>
+      <c r="E127" t="s">
+        <v>334</v>
+      </c>
       <c r="F127" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.txtNombre=Ingrese el nombre</v>
       </c>
       <c r="G127" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.txtNombre=</v>
+        <v>RegistroPaquetesController.txtNombre=Enter name</v>
       </c>
       <c r="H127" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6173,13 +6914,16 @@
       <c r="D128" t="s">
         <v>198</v>
       </c>
+      <c r="E128" t="s">
+        <v>353</v>
+      </c>
       <c r="F128" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblDuracion=Duracion en dias:</v>
       </c>
       <c r="G128" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblDuracion=</v>
+        <v>RegistroPaquetesController.lblDuracion=Duration in days:</v>
       </c>
       <c r="H128" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6212,13 +6956,16 @@
       <c r="D129" t="s">
         <v>199</v>
       </c>
+      <c r="E129" t="s">
+        <v>354</v>
+      </c>
       <c r="F129" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.txtDuracion=Ingrese la duracion del paquete</v>
       </c>
       <c r="G129" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.txtDuracion=</v>
+        <v>RegistroPaquetesController.txtDuracion=Enter the duration of the package</v>
       </c>
       <c r="H129" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6251,13 +6998,16 @@
       <c r="D130" t="s">
         <v>200</v>
       </c>
+      <c r="E130" t="s">
+        <v>355</v>
+      </c>
       <c r="F130" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblServicios=Servicios adicionales:</v>
       </c>
       <c r="G130" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblServicios=</v>
+        <v>RegistroPaquetesController.lblServicios=Additional services:</v>
       </c>
       <c r="H130" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6290,13 +7040,16 @@
       <c r="D131" t="s">
         <v>201</v>
       </c>
+      <c r="E131" t="s">
+        <v>356</v>
+      </c>
       <c r="F131" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.txtServicios=Ingrese los servicios adicionales</v>
       </c>
       <c r="G131" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.txtServicios=</v>
+        <v>RegistroPaquetesController.txtServicios=Enter the additional services</v>
       </c>
       <c r="H131" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6329,13 +7082,16 @@
       <c r="D132" t="s">
         <v>202</v>
       </c>
+      <c r="E132" t="s">
+        <v>357</v>
+      </c>
       <c r="F132" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblPrecio=Precio:</v>
       </c>
       <c r="G132" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblPrecio=</v>
+        <v>RegistroPaquetesController.lblPrecio=Price in days:</v>
       </c>
       <c r="H132" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6368,13 +7124,16 @@
       <c r="D133" t="s">
         <v>203</v>
       </c>
+      <c r="E133" t="s">
+        <v>358</v>
+      </c>
       <c r="F133" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.txtPrecio=Digite el precio</v>
       </c>
       <c r="G133" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.txtPrecio=</v>
+        <v>RegistroPaquetesController.txtPrecio=Enter the price</v>
       </c>
       <c r="H133" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6407,13 +7166,16 @@
       <c r="D134" t="s">
         <v>204</v>
       </c>
+      <c r="E134" t="s">
+        <v>359</v>
+      </c>
       <c r="F134" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblCupo=Cupo maximo:</v>
       </c>
       <c r="G134" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblCupo=</v>
+        <v>RegistroPaquetesController.lblCupo=Maximum quota:</v>
       </c>
       <c r="H134" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6446,13 +7208,16 @@
       <c r="D135" t="s">
         <v>205</v>
       </c>
+      <c r="E135" t="s">
+        <v>360</v>
+      </c>
       <c r="F135" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.txtCupo=Digite el cupo maximo</v>
       </c>
       <c r="G135" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.txtCupo=</v>
+        <v>RegistroPaquetesController.txtCupo=Enter the maximum quota</v>
       </c>
       <c r="H135" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6485,13 +7250,16 @@
       <c r="D136" t="s">
         <v>206</v>
       </c>
+      <c r="E136" t="s">
+        <v>312</v>
+      </c>
       <c r="F136" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblFechaInicio=Fecha inicio:</v>
       </c>
       <c r="G136" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblFechaInicio=</v>
+        <v>RegistroPaquetesController.lblFechaInicio=Start date:</v>
       </c>
       <c r="H136" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6524,13 +7292,16 @@
       <c r="D137" t="s">
         <v>207</v>
       </c>
+      <c r="E137" t="s">
+        <v>361</v>
+      </c>
       <c r="F137" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.dpInicio=Ingrese la fecha de inicio del paquete</v>
       </c>
       <c r="G137" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.dpInicio=</v>
+        <v>RegistroPaquetesController.dpInicio=Enter the start date of the package</v>
       </c>
       <c r="H137" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6563,13 +7334,16 @@
       <c r="D138" t="s">
         <v>208</v>
       </c>
+      <c r="E138" t="s">
+        <v>362</v>
+      </c>
       <c r="F138" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblFechaFin=Fecha fin:</v>
       </c>
       <c r="G138" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblFechaFin=</v>
+        <v>RegistroPaquetesController.lblFechaFin=End date:</v>
       </c>
       <c r="H138" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6602,13 +7376,16 @@
       <c r="D139" t="s">
         <v>209</v>
       </c>
+      <c r="E139" t="s">
+        <v>363</v>
+      </c>
       <c r="F139" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.dpFin=Ingrese la fecha de finalizacion del paquete</v>
       </c>
       <c r="G139" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.dpFin=</v>
+        <v>RegistroPaquetesController.dpFin=Enter the end date of the package</v>
       </c>
       <c r="H139" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6641,13 +7418,16 @@
       <c r="D140" t="s">
         <v>210</v>
       </c>
+      <c r="E140" t="s">
+        <v>364</v>
+      </c>
       <c r="F140" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.lblSeleccionar=Seleccione los destinos que va a contener el paquete</v>
       </c>
       <c r="G140" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.lblSeleccionar=</v>
+        <v>RegistroPaquetesController.lblSeleccionar=Select the destinations that the package will contain</v>
       </c>
       <c r="H140" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6680,13 +7460,16 @@
       <c r="D141" t="s">
         <v>32</v>
       </c>
+      <c r="E141" t="s">
+        <v>32</v>
+      </c>
       <c r="F141" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.colId=ID</v>
       </c>
       <c r="G141" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.colId=</v>
+        <v>RegistroPaquetesController.colId=ID</v>
       </c>
       <c r="H141" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6719,13 +7502,16 @@
       <c r="D142" t="s">
         <v>211</v>
       </c>
+      <c r="E142" t="s">
+        <v>365</v>
+      </c>
       <c r="F142" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.colNombre=NOMBRE</v>
       </c>
       <c r="G142" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.colNombre=</v>
+        <v>RegistroPaquetesController.colNombre=NAME</v>
       </c>
       <c r="H142" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6758,13 +7544,16 @@
       <c r="D143" t="s">
         <v>212</v>
       </c>
+      <c r="E143" t="s">
+        <v>366</v>
+      </c>
       <c r="F143" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.colCiudad=CIUDAD</v>
       </c>
       <c r="G143" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.colCiudad=</v>
+        <v>RegistroPaquetesController.colCiudad=CITY</v>
       </c>
       <c r="H143" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6797,13 +7586,16 @@
       <c r="D144" t="s">
         <v>213</v>
       </c>
+      <c r="E144" t="s">
+        <v>367</v>
+      </c>
       <c r="F144" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.colDescripcion=DESCRIPCION</v>
       </c>
       <c r="G144" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.colDescripcion=</v>
+        <v>RegistroPaquetesController.colDescripcion=DESCRIPTION</v>
       </c>
       <c r="H144" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6836,13 +7628,16 @@
       <c r="D145" t="s">
         <v>214</v>
       </c>
+      <c r="E145" t="s">
+        <v>368</v>
+      </c>
       <c r="F145" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.colClima=CLIMA</v>
       </c>
       <c r="G145" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.colClima=</v>
+        <v>RegistroPaquetesController.colClima=WEATHER</v>
       </c>
       <c r="H145" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6875,13 +7670,16 @@
       <c r="D146" t="s">
         <v>32</v>
       </c>
+      <c r="E146" t="s">
+        <v>32</v>
+      </c>
       <c r="F146" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.colIdSelect=ID</v>
       </c>
       <c r="G146" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.colIdSelect=</v>
+        <v>RegistroPaquetesController.colIdSelect=ID</v>
       </c>
       <c r="H146" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6914,13 +7712,16 @@
       <c r="D147" t="s">
         <v>211</v>
       </c>
+      <c r="E147" t="s">
+        <v>365</v>
+      </c>
       <c r="F147" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>RegistroPaquetesController.colNombreSelect=NOMBRE</v>
       </c>
       <c r="G147" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>RegistroPaquetesController.colNombreSelect=</v>
+        <v>RegistroPaquetesController.colNombreSelect=NAME</v>
       </c>
       <c r="H147" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6953,13 +7754,16 @@
       <c r="D148" t="s">
         <v>230</v>
       </c>
+      <c r="E148" t="s">
+        <v>369</v>
+      </c>
       <c r="F148" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.lblTitle=GESTIONAR SOLICITUDES GUIAS</v>
       </c>
       <c r="G148" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.lblTitle=</v>
+        <v>SolicitudGuiaController.lblTitle=MANAGE GUIDE REQUESTS</v>
       </c>
       <c r="H148" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -6992,13 +7796,16 @@
       <c r="D149" t="s">
         <v>43</v>
       </c>
+      <c r="E149" t="s">
+        <v>278</v>
+      </c>
       <c r="F149" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.txtBuscar=Buscar</v>
       </c>
       <c r="G149" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.txtBuscar=</v>
+        <v>SolicitudGuiaController.txtBuscar=Search</v>
       </c>
       <c r="H149" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7031,13 +7838,16 @@
       <c r="D150" t="s">
         <v>27</v>
       </c>
+      <c r="E150" t="s">
+        <v>269</v>
+      </c>
       <c r="F150" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.colNombre=Nombre</v>
       </c>
       <c r="G150" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.colNombre=</v>
+        <v>SolicitudGuiaController.colNombre=Name</v>
       </c>
       <c r="H150" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7070,13 +7880,16 @@
       <c r="D151" t="s">
         <v>26</v>
       </c>
+      <c r="E151" t="s">
+        <v>32</v>
+      </c>
       <c r="F151" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.colIdentificacion=Identificacion</v>
       </c>
       <c r="G151" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.colIdentificacion=</v>
+        <v>SolicitudGuiaController.colIdentificacion=ID</v>
       </c>
       <c r="H151" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7109,13 +7922,16 @@
       <c r="D152" t="s">
         <v>61</v>
       </c>
+      <c r="E152" t="s">
+        <v>285</v>
+      </c>
       <c r="F152" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.colHorasExperiencia=Horas de experiencia</v>
       </c>
       <c r="G152" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.colHorasExperiencia=</v>
+        <v>SolicitudGuiaController.colHorasExperiencia=Hours of experience</v>
       </c>
       <c r="H152" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7148,13 +7964,16 @@
       <c r="D153" t="s">
         <v>25</v>
       </c>
+      <c r="E153" t="s">
+        <v>267</v>
+      </c>
       <c r="F153" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.colIdiomas=Idiomas</v>
       </c>
       <c r="G153" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.colIdiomas=</v>
+        <v>SolicitudGuiaController.colIdiomas=Languages</v>
       </c>
       <c r="H153" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7187,13 +8006,16 @@
       <c r="D154" t="s">
         <v>231</v>
       </c>
+      <c r="E154" t="s">
+        <v>370</v>
+      </c>
       <c r="F154" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.btnAceptar=ACEPTAR</v>
       </c>
       <c r="G154" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.btnAceptar=</v>
+        <v>SolicitudGuiaController.btnAceptar=ACCEPT</v>
       </c>
       <c r="H154" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7226,13 +8048,16 @@
       <c r="D155" t="s">
         <v>232</v>
       </c>
+      <c r="E155" t="s">
+        <v>371</v>
+      </c>
       <c r="F155" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>SolicitudGuiaController.btnDenegar=DENEGAR</v>
       </c>
       <c r="G155" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>SolicitudGuiaController.btnDenegar=</v>
+        <v>SolicitudGuiaController.btnDenegar=DENY</v>
       </c>
       <c r="H155" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7265,13 +8090,16 @@
       <c r="D156" t="s">
         <v>95</v>
       </c>
+      <c r="E156" t="s">
+        <v>297</v>
+      </c>
       <c r="F156" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ViewDestinosController.lblTitle=Destinos</v>
       </c>
       <c r="G156" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ViewDestinosController.lblTitle=</v>
+        <v>ViewDestinosController.lblTitle=Destinations</v>
       </c>
       <c r="H156" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7304,13 +8132,16 @@
       <c r="D157" t="s">
         <v>94</v>
       </c>
+      <c r="E157" t="s">
+        <v>298</v>
+      </c>
       <c r="F157" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>ViewPaquetesController.lblTitle=Paquetes</v>
       </c>
       <c r="G157" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>ViewPaquetesController.lblTitle=</v>
+        <v>ViewPaquetesController.lblTitle=Packages</v>
       </c>
       <c r="H157" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7343,13 +8174,16 @@
       <c r="D158" t="s">
         <v>249</v>
       </c>
+      <c r="E158" t="s">
+        <v>372</v>
+      </c>
       <c r="F158" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>EstadisticasController.lblTitle=ESTADÍSTICAS</v>
       </c>
       <c r="G158" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>EstadisticasController.lblTitle=</v>
+        <v>EstadisticasController.lblTitle=STATISTICS</v>
       </c>
       <c r="H158" s="1" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7382,13 +8216,16 @@
       <c r="D159" t="s">
         <v>251</v>
       </c>
+      <c r="E159" t="s">
+        <v>373</v>
+      </c>
       <c r="F159" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>EstadisticasController.lblDestinosReservados=DESTINOS MAS RESERVADOS</v>
       </c>
       <c r="G159" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>EstadisticasController.lblDestinosReservados=</v>
+        <v>EstadisticasController.lblDestinosReservados=MOST BOOKED DESTINATIONS</v>
       </c>
       <c r="H159" s="1" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7421,13 +8258,16 @@
       <c r="D160" t="s">
         <v>253</v>
       </c>
+      <c r="E160" t="s">
+        <v>374</v>
+      </c>
       <c r="F160" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>EstadisticasController.lblDestinosBuscados=DESTINOS MAS BUSCADOS</v>
       </c>
       <c r="G160" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>EstadisticasController.lblDestinosBuscados=</v>
+        <v>EstadisticasController.lblDestinosBuscados=MOST SEARCHED DESTINATIONS</v>
       </c>
       <c r="H160" s="1" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7460,13 +8300,16 @@
       <c r="D161" t="s">
         <v>257</v>
       </c>
+      <c r="E161" t="s">
+        <v>375</v>
+      </c>
       <c r="F161" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>EstadisticasController.lblGuiasPuntuados=GUIAS MEJOR PUNTUADOS</v>
       </c>
       <c r="G161" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>EstadisticasController.lblGuiasPuntuados=</v>
+        <v>EstadisticasController.lblGuiasPuntuados=TOP RATED GUIDES</v>
       </c>
       <c r="H161" s="1" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7499,13 +8342,16 @@
       <c r="D162" t="s">
         <v>256</v>
       </c>
+      <c r="E162" t="s">
+        <v>376</v>
+      </c>
       <c r="F162" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
         <v>EstadisticasController.lblPaquetesReservados=PAQUETES MAS RESERVADOS</v>
       </c>
       <c r="G162" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
-        <v>EstadisticasController.lblPaquetesReservados=</v>
+        <v>EstadisticasController.lblPaquetesReservados=MOST BOOKED PACKAGES</v>
       </c>
       <c r="H162" s="1" t="str">
         <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
@@ -7522,6 +8368,48 @@
       <c r="K162" s="1" t="str">
         <f>CONCATENATE(Tabla1[[#This Row],[ID]],".setPromptText(",Tabla1[[#This Row],[Bundle]],");")</f>
         <v>lblPaquetesReservados.setPromptText(bundle.getString("EstadisticasController.lblPaquetesReservados"));</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>377</v>
+      </c>
+      <c r="B163" t="s">
+        <v>378</v>
+      </c>
+      <c r="C163" s="1" t="str">
+        <f>CONCATENATE(A163,".",B163)</f>
+        <v>GuiaTuristicoController.txtDescription</v>
+      </c>
+      <c r="D163" t="s">
+        <v>379</v>
+      </c>
+      <c r="E163" t="s">
+        <v>380</v>
+      </c>
+      <c r="F163" s="1" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[Español]])</f>
+        <v>GuiaTuristicoController.txtDescription=Idiomas Hablados: %s\nExp Horas: %d</v>
+      </c>
+      <c r="G163" s="1" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[Codigo]],"=",Tabla1[[#This Row],[English]])</f>
+        <v>GuiaTuristicoController.txtDescription=Languages Spoken: %s\nHours: %d</v>
+      </c>
+      <c r="H163" s="1" t="str">
+        <f>CONCATENATE("bundle.getString(",Tabla1[[#This Row],[Comilla]],Tabla1[[#This Row],[Codigo]],Tabla1[[#This Row],[Comilla]],")")</f>
+        <v>bundle.getString("GuiaTuristicoController.txtDescription")</v>
+      </c>
+      <c r="I163" s="1" t="str">
+        <f>""""</f>
+        <v>"</v>
+      </c>
+      <c r="J163" s="1" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[ID]],".setText(",Tabla1[[#This Row],[Bundle]],");")</f>
+        <v>txtDescription.setText(bundle.getString("GuiaTuristicoController.txtDescription"));</v>
+      </c>
+      <c r="K163" s="1" t="str">
+        <f>CONCATENATE(Tabla1[[#This Row],[ID]],".setPromptText(",Tabla1[[#This Row],[Bundle]],");")</f>
+        <v>txtDescription.setPromptText(bundle.getString("GuiaTuristicoController.txtDescription"));</v>
       </c>
     </row>
   </sheetData>

</xml_diff>